<commit_message>
Added tests to oardAdjTargetsTests.java
</commit_message>
<xml_diff>
--- a/ClueGame/C14 Layout.xlsx
+++ b/ClueGame/C14 Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\workspace\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\C12paths\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -136,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,7 +199,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,23 +319,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,12 +619,12 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -692,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -766,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -840,8 +846,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -859,7 +865,7 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -868,7 +874,7 @@
       <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -886,13 +892,13 @@
       <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -914,8 +920,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -930,7 +936,7 @@
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -978,7 +984,7 @@
       <c r="U5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="W5" s="1" t="s">
@@ -988,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1052,7 @@
       <c r="S6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T6" s="17" t="s">
+      <c r="T6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="U6" s="1" t="s">
@@ -1062,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1284,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1345,7 @@
       <c r="R10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T10" s="2" t="s">
@@ -1358,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1425,15 +1431,15 @@
       <c r="V11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W11" s="16" t="s">
+      <c r="W11" s="13" t="s">
         <v>0</v>
       </c>
       <c r="X11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1506,7 +1512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1570,7 @@
       <c r="S13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="T13" s="11" t="s">
         <v>0</v>
       </c>
       <c r="U13" s="2" t="s">
@@ -1580,7 +1586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1599,7 @@
       <c r="D14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1654,7 +1660,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1703,7 +1709,7 @@
       <c r="P15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" s="18" t="s">
         <v>2</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1718,7 +1724,7 @@
       <c r="U15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="V15" s="18" t="s">
         <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
@@ -1728,7 +1734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1802,14 +1808,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1876,7 +1882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1950,8 +1956,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1978,10 +1984,10 @@
       <c r="I19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="11" t="s">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="s">
@@ -1993,7 +1999,7 @@
       <c r="N19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="P19" s="1" t="s">
@@ -2024,7 +2030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2040,7 +2046,7 @@
       <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -2098,7 +2104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2172,7 +2178,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -2215,7 +2221,7 @@
       <c r="N22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O22" s="16" t="s">
+      <c r="O22" s="13" t="s">
         <v>2</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -2246,7 +2252,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2317,69 +2323,69 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="18"/>
-      <c r="E25" s="19" t="s">
+    <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="15"/>
+      <c r="E25" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="20"/>
-    </row>
-    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="6" t="s">
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="17"/>
+    </row>
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="7"/>
-      <c r="E27" s="6" t="s">
+    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="6"/>
+      <c r="E27" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D28" s="8"/>
-      <c r="E28" s="6" t="s">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D28" s="7"/>
+      <c r="E28" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D29" s="9"/>
-      <c r="E29" s="6" t="s">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+      <c r="E29" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D30" s="10"/>
-      <c r="E30" s="6" t="s">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D30" s="9"/>
+      <c r="E30" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D31" s="11"/>
-      <c r="E31" s="6" t="s">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D31" s="10"/>
+      <c r="E31" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="21"/>
-      <c r="E32" s="6" t="s">
+    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="20"/>
+      <c r="E32" s="5" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more tests for ClueGame
</commit_message>
<xml_diff>
--- a/ClueGame/C14 Layout.xlsx
+++ b/ClueGame/C14 Layout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="35">
   <si>
     <t>P</t>
   </si>
@@ -95,12 +95,6 @@
     <t>White: Locations with only walkways as adjacent locations</t>
   </si>
   <si>
-    <t>Orange: Locations within rooms (should have empty adjacency list)</t>
-  </si>
-  <si>
-    <t>Purple: Locations that are at each edge of the board</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marron: Locatons that are adjacent to a doorway with needed directions(i.e., the adjacency list will include the doorway). Test all four directions. </t>
   </si>
   <si>
@@ -114,6 +108,27 @@
   </si>
   <si>
     <t>Number of doors = 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purple: Locations for testing walkway adjacencies </t>
+  </si>
+  <si>
+    <t>testAdjacenciesInsideRooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange: Locations tested for one step </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testTargetsOneStep </t>
+  </si>
+  <si>
+    <t>testTarrgetsTwoSteps</t>
+  </si>
+  <si>
+    <t>testTarrgetsFourSteps</t>
+  </si>
+  <si>
+    <t>testTargetsSixSteps</t>
   </si>
 </sst>
 </file>
@@ -136,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +221,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -322,9 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -336,12 +367,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC00CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -616,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+      <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +678,7 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -658,7 +702,7 @@
       <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -682,7 +726,7 @@
       <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -695,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="X1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -769,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="X2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -830,7 +874,7 @@
       <c r="S3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="U3" s="1" t="s">
@@ -843,11 +887,11 @@
         <v>3</v>
       </c>
       <c r="X3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -865,7 +909,7 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -874,7 +918,7 @@
       <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -892,13 +936,13 @@
       <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -917,81 +961,81 @@
         <v>3</v>
       </c>
       <c r="X4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V5" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X5">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1052,7 +1096,7 @@
       <c r="S6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="12" t="s">
         <v>0</v>
       </c>
       <c r="U6" s="1" t="s">
@@ -1065,11 +1109,11 @@
         <v>3</v>
       </c>
       <c r="X6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1139,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="X7">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1200,11 +1244,11 @@
       <c r="S8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>3</v>
@@ -1213,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="X8">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1287,7 +1331,7 @@
         <v>3</v>
       </c>
       <c r="X9">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1357,11 +1401,11 @@
       <c r="V10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="20" t="s">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1380,7 +1424,7 @@
       <c r="E11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1431,11 +1475,11 @@
       <c r="V11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W11" s="13" t="s">
+      <c r="W11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X11">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1509,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="X12">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1570,7 +1614,7 @@
       <c r="S13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="11" t="s">
+      <c r="T13" s="9" t="s">
         <v>0</v>
       </c>
       <c r="U13" s="2" t="s">
@@ -1583,11 +1627,11 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1641,7 +1685,7 @@
       <c r="R14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="S14" s="11" t="s">
         <v>0</v>
       </c>
       <c r="T14" s="3" t="s">
@@ -1657,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="X14">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -1709,7 +1753,7 @@
       <c r="P15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="18" t="s">
+      <c r="Q15" s="16" t="s">
         <v>2</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1724,14 +1768,14 @@
       <c r="U15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V15" s="18" t="s">
+      <c r="V15" s="16" t="s">
         <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="X15">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -1756,7 +1800,7 @@
       <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="10" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1805,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="X16">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
@@ -1815,7 +1859,7 @@
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1879,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="X17">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -1953,11 +1997,11 @@
         <v>1</v>
       </c>
       <c r="X18">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1984,10 +2028,10 @@
       <c r="I19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="9" t="s">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="s">
@@ -1999,7 +2043,7 @@
       <c r="N19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O19" s="12" t="s">
+      <c r="O19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P19" s="1" t="s">
@@ -2027,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="X19">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -2046,7 +2090,7 @@
       <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -2101,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="X20">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -2175,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="X21">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -2191,7 +2235,7 @@
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2212,7 +2256,7 @@
       <c r="K22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="25" t="s">
         <v>0</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -2221,7 +2265,7 @@
       <c r="N22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O22" s="13" t="s">
+      <c r="O22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -2230,10 +2274,10 @@
       <c r="Q22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2" t="s">
+      <c r="R22" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="27" t="s">
         <v>0</v>
       </c>
       <c r="T22" s="1" t="s">
@@ -2249,103 +2293,103 @@
         <v>1</v>
       </c>
       <c r="X22">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
         <v>4</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>5</v>
       </c>
-      <c r="F23">
-        <v>6</v>
-      </c>
       <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
         <v>7</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>8</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>9</v>
       </c>
-      <c r="J23">
-        <v>10</v>
-      </c>
       <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
         <v>11</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>12</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>13</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>14</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>15</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>16</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>17</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>18</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>19</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>20</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>21</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>22</v>
-      </c>
-      <c r="W23">
-        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="15"/>
-      <c r="E25" s="16" t="s">
+      <c r="D25" s="13"/>
+      <c r="E25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="17"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2353,35 +2397,59 @@
       <c r="E27" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="7"/>
       <c r="E28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="22"/>
+      <c r="E29" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="8"/>
+      <c r="E30" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="23"/>
+      <c r="E31" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D29" s="8"/>
-      <c r="E29" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D30" s="9"/>
-      <c r="E30" s="5" t="s">
+    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="18"/>
+      <c r="E32" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D31" s="10"/>
-      <c r="E31" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="20"/>
-      <c r="E32" s="5" t="s">
-        <v>28</v>
+    <row r="33" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="21"/>
+      <c r="T33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D34" s="24"/>
+      <c r="T34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D35" s="26"/>
+      <c r="T35" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more tests and updated excel diagram of the board
</commit_message>
<xml_diff>
--- a/ClueGame/C14 Layout.xlsx
+++ b/ClueGame/C14 Layout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="46">
   <si>
     <t>P</t>
   </si>
@@ -92,33 +92,15 @@
     <t>Key</t>
   </si>
   <si>
-    <t>White: Locations with only walkways as adjacent locations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marron: Locatons that are adjacent to a doorway with needed directions(i.e., the adjacency list will include the doorway). Test all four directions. </t>
-  </si>
-  <si>
-    <t>Green: Locations that are beside a room cell that is not a doorway</t>
-  </si>
-  <si>
     <t>HL</t>
   </si>
   <si>
-    <t>Grey: Locations that are doorways( should have only one adjacent cell)</t>
-  </si>
-  <si>
     <t>Number of doors = 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Purple: Locations for testing walkway adjacencies </t>
-  </si>
-  <si>
     <t>testAdjacenciesInsideRooms</t>
   </si>
   <si>
-    <t xml:space="preserve">Orange: Locations tested for one step </t>
-  </si>
-  <si>
     <t xml:space="preserve">testTargetsOneStep </t>
   </si>
   <si>
@@ -129,13 +111,64 @@
   </si>
   <si>
     <t>testTargetsSixSteps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testTargetsIntoRoom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testAdjacencyRoomExit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testAdjacencyDoorways </t>
+  </si>
+  <si>
+    <t>testAdjacncyWalkways</t>
+  </si>
+  <si>
+    <t>testRoomExit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations used ot test the potential targets for a player on the pathway </t>
+  </si>
+  <si>
+    <t>Locations used to test movement inside rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations used to test exiting room through doorway </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations used to test entry into room through doorway </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations used to test the potentaial targets for a player who can more four steps </t>
+  </si>
+  <si>
+    <t>Locations used to test the potential targets of a player who can move two steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations used to test the potential targets of a player who can move one step </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location used to test the potential targets for a player who can move six steps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location used to test entering a room from exactly two teps away </t>
+  </si>
+  <si>
+    <t>testTargetsIntoRoomShortcut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location used to test entry into a room where it takes less steps than the pathlength to enter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location used to test the potential targets as a player leaves the room for one and two steps </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +183,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,12 +242,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -239,6 +273,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC00CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,26 +407,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,6 +439,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FFCC"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCC3300"/>
+      <color rgb="FF000066"/>
+      <color rgb="FFFF7C80"/>
       <color rgb="FFCC00CC"/>
     </mruColors>
   </colors>
@@ -660,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +739,7 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -702,7 +763,7 @@
       <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -726,7 +787,7 @@
       <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -856,7 +917,7 @@
       <c r="M3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -874,7 +935,7 @@
       <c r="S3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="U3" s="1" t="s">
@@ -891,7 +952,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -909,7 +970,7 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="15" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -918,7 +979,7 @@
       <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -942,7 +1003,7 @@
       <c r="Q4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="R4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -965,13 +1026,13 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="30" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -980,7 +1041,7 @@
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1028,7 +1089,7 @@
       <c r="U5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="V5" s="14" t="s">
         <v>3</v>
       </c>
       <c r="W5" s="1" t="s">
@@ -1096,7 +1157,7 @@
       <c r="S6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T6" s="12" t="s">
+      <c r="T6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="U6" s="1" t="s">
@@ -1113,7 +1174,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1244,11 +1305,11 @@
       <c r="S8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="T8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>3</v>
@@ -1401,7 +1462,7 @@
       <c r="V10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W10" s="20" t="s">
+      <c r="W10" s="18" t="s">
         <v>0</v>
       </c>
       <c r="X10">
@@ -1424,7 +1485,7 @@
       <c r="E11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1614,7 +1675,7 @@
       <c r="S13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="9" t="s">
+      <c r="T13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="U13" s="2" t="s">
@@ -1631,7 +1692,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1685,7 +1746,7 @@
       <c r="R14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="S14" s="10" t="s">
         <v>0</v>
       </c>
       <c r="T14" s="3" t="s">
@@ -1753,7 +1814,7 @@
       <c r="P15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="16" t="s">
+      <c r="Q15" s="14" t="s">
         <v>2</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1768,7 +1829,7 @@
       <c r="U15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V15" s="16" t="s">
+      <c r="V15" s="14" t="s">
         <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
@@ -1800,7 +1861,7 @@
       <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1815,7 +1876,7 @@
       <c r="L16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="24" t="s">
         <v>0</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -1859,7 +1920,7 @@
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -2028,10 +2089,10 @@
       <c r="I19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="8" t="s">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="s">
@@ -2090,7 +2151,7 @@
       <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -2235,7 +2296,7 @@
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2256,7 +2317,7 @@
       <c r="K22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L22" s="25" t="s">
+      <c r="L22" s="22" t="s">
         <v>0</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -2274,10 +2335,10 @@
       <c r="Q22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R22" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="27" t="s">
+      <c r="R22" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="23" t="s">
         <v>0</v>
       </c>
       <c r="T22" s="1" t="s">
@@ -2369,87 +2430,126 @@
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="13"/>
-      <c r="E25" s="14" t="s">
+      <c r="D25" s="11"/>
+      <c r="E25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="15"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="13"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="6"/>
       <c r="E27" s="5" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="T27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="7"/>
       <c r="E28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="20"/>
+      <c r="E29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="21"/>
+      <c r="E30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="16"/>
+      <c r="E31" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T31" t="s">
         <v>30</v>
       </c>
-      <c r="T28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="22"/>
-      <c r="E29" s="5" t="s">
+    </row>
+    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="19"/>
+      <c r="E32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="26"/>
+      <c r="E33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="28"/>
+      <c r="E34" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="8"/>
-      <c r="E30" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="23"/>
-      <c r="E31" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="18"/>
-      <c r="E32" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="21"/>
-      <c r="T33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D34" s="24"/>
-      <c r="T34" t="s">
+    <row r="35" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="27"/>
+      <c r="E35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="29"/>
+      <c r="E36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="26"/>
-      <c r="T35" t="s">
-        <v>34</v>
+    <row r="37" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="31"/>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="T37" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>